<commit_message>
Update ids for Hypertension workflow.
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/Documents/HTN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22245985-C59A-9D41-BDFF-298C1EDB3404}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBC4F8F8-AEED-A447-A761-6576C860370D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
   <sheets>
-    <sheet name="Initial Diagnosis (ID)" sheetId="1" r:id="rId1"/>
+    <sheet name="Hypertension Initial Dx (H)" sheetId="1" r:id="rId1"/>
     <sheet name="Monitoring (M)" sheetId="2" r:id="rId2"/>
     <sheet name="NonPharma Interventions (NPI)" sheetId="4" r:id="rId3"/>
     <sheet name="Pharma Interventions (PI)" sheetId="3" r:id="rId4"/>
@@ -74,27 +74,6 @@
     <t>Pregnant</t>
   </si>
   <si>
-    <t>ID-ExcludedOver80</t>
-  </si>
-  <si>
-    <t>ID-ExcludedUnder18</t>
-  </si>
-  <si>
-    <t>ID-ExcludedPregnant</t>
-  </si>
-  <si>
-    <t>ID-ExcludedEndStageRenalDisease</t>
-  </si>
-  <si>
-    <t>ID-ExcludedNormalBP</t>
-  </si>
-  <si>
-    <t>ID-HypertensiveEmergencySBP</t>
-  </si>
-  <si>
-    <t>ID-HypertensiveEmergencyDBP</t>
-  </si>
-  <si>
     <t>End Stage Renal Disease</t>
   </si>
   <si>
@@ -119,9 +98,6 @@
     <t>Condition</t>
   </si>
   <si>
-    <t>ID-MonitoringPreexistingHTN</t>
-  </si>
-  <si>
     <t>Hypertension</t>
   </si>
   <si>
@@ -143,12 +119,6 @@
     <t>Set Avg &gt; 160 SBP</t>
   </si>
   <si>
-    <t>ID-ConsiderHTNStage2</t>
-  </si>
-  <si>
-    <t>ID-ConsiderHTNStage1</t>
-  </si>
-  <si>
     <t>Last BP AND Set Avg &gt; 130/80</t>
   </si>
   <si>
@@ -176,18 +146,9 @@
     <t>Consider HTN Stage 1</t>
   </si>
   <si>
-    <t>ID-HTNStage2LastBP</t>
-  </si>
-  <si>
-    <t>ID-HTNStage2AverageBP</t>
-  </si>
-  <si>
     <t>Last BP OR Set Avg &gt; 130/80</t>
   </si>
   <si>
-    <t>ID-PrescribeHBPABPMonitoring</t>
-  </si>
-  <si>
     <t>Prescribe HBP or ABP Monitoring</t>
   </si>
   <si>
@@ -206,9 +167,6 @@
     <t>Prescribe Ambulatory BP Monitoring</t>
   </si>
   <si>
-    <t>ID-PrescribeAmbulatoryBPMonitoring</t>
-  </si>
-  <si>
     <t>SBP Coeff of Var &gt; 11 for all BPs and no ABPM</t>
   </si>
   <si>
@@ -218,9 +176,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>ID-NoFurtherAction</t>
-  </si>
-  <si>
     <t>M-RecommendMoreBPsMissingData</t>
   </si>
   <si>
@@ -266,9 +221,6 @@
     <t>M-PatientAtGoal</t>
   </si>
   <si>
-    <t>ID-RecommendMoreBPs</t>
-  </si>
-  <si>
     <t>M-RecommendHBPABPMonitoring</t>
   </si>
   <si>
@@ -513,6 +465,54 @@
   </si>
   <si>
     <t>NOT "Patient at BP Goal"</t>
+  </si>
+  <si>
+    <t>H-ExcludedUnder18</t>
+  </si>
+  <si>
+    <t>H-ExcludedPregnant</t>
+  </si>
+  <si>
+    <t>H-ExcludedEndStageRenalDisease</t>
+  </si>
+  <si>
+    <t>H-ExcludedNormalBP</t>
+  </si>
+  <si>
+    <t>H-HypertensiveEmergencySBP</t>
+  </si>
+  <si>
+    <t>H-HypertensiveEmergencyDBP</t>
+  </si>
+  <si>
+    <t>H-MonitoringPreexistingHTN</t>
+  </si>
+  <si>
+    <t>H-RecommendMoreBPs</t>
+  </si>
+  <si>
+    <t>H-HTNStage2LastBP</t>
+  </si>
+  <si>
+    <t>H-HTNStage2AverageBP</t>
+  </si>
+  <si>
+    <t>H-ConsiderHTNStage2</t>
+  </si>
+  <si>
+    <t>H-ConsiderHTNStage1</t>
+  </si>
+  <si>
+    <t>H-PrescribeHBPABPMonitoring</t>
+  </si>
+  <si>
+    <t>H-PrescribeAmbulatoryBPMonitoring</t>
+  </si>
+  <si>
+    <t>H-NoFurtherAction</t>
+  </si>
+  <si>
+    <t>H-ExcludedOver80</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1053,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1070,10 +1070,10 @@
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -1088,31 +1088,31 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>12</v>
@@ -1123,52 +1123,52 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>15</v>
+        <v>145</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>13</v>
@@ -1177,28 +1177,28 @@
     <row r="5" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="G5" s="5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>6</v>
@@ -1215,37 +1215,37 @@
         <v>0</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="12" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -1253,42 +1253,42 @@
         <v>11</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>29</v>
+        <v>151</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H10" s="17" t="b">
         <v>0</v>
@@ -1296,96 +1296,96 @@
     </row>
     <row r="11" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>49</v>
+        <v>154</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P12" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="P12" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>37</v>
+        <v>155</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H13" s="20" t="b">
         <v>1</v>
@@ -1405,22 +1405,22 @@
     </row>
     <row r="14" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H14" s="13" t="b">
         <v>1</v>
@@ -1437,22 +1437,22 @@
     </row>
     <row r="15" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>51</v>
+        <v>157</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H15" s="20" t="b">
         <v>1</v>
@@ -1472,22 +1472,22 @@
     </row>
     <row r="16" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>58</v>
+        <v>158</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H16" s="13" t="b">
         <v>1</v>
@@ -1510,22 +1510,22 @@
     </row>
     <row r="17" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>62</v>
+        <v>159</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H17" s="20" t="b">
         <v>1</v>
@@ -1577,10 +1577,10 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -1595,25 +1595,25 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="Q1" s="21" t="s">
         <v>12</v>
@@ -1624,51 +1624,51 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q2" s="22"/>
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q3" s="23"/>
     </row>
     <row r="4" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>13</v>
@@ -1678,29 +1678,29 @@
     <row r="5" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="Q5" s="23"/>
     </row>
     <row r="6" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>6</v>
@@ -1716,43 +1716,43 @@
     <row r="7" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="Q7" s="24"/>
     </row>
     <row r="8" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="H8" s="20" t="b">
         <v>0</v>
@@ -1761,25 +1761,25 @@
     </row>
     <row r="9" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="H9" s="13" t="b">
         <v>1</v>
@@ -1791,25 +1791,25 @@
     </row>
     <row r="10" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="H10" s="10" t="b">
         <v>1</v>
@@ -1825,22 +1825,22 @@
     <row r="11" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="H11" s="12" t="b">
         <v>1</v>
@@ -1858,25 +1858,25 @@
     </row>
     <row r="12" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="H12" s="13" t="b">
         <v>1</v>
@@ -1897,25 +1897,25 @@
     </row>
     <row r="13" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="H13" s="20" t="b">
         <v>1</v>
@@ -1939,25 +1939,25 @@
     </row>
     <row r="14" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="H14" s="13" t="b">
         <v>1</v>
@@ -2010,10 +2010,10 @@
   <sheetData>
     <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -2022,28 +2022,28 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="M1" s="21" t="s">
         <v>12</v>
@@ -2054,89 +2054,89 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="M2" s="22"/>
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="M3" s="23"/>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="M4" s="23"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="M5" s="23"/>
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="M6" s="24"/>
     </row>
     <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F7" s="10" t="b">
         <v>0</v>
@@ -2145,19 +2145,19 @@
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F8" s="3" t="b">
         <v>1</v>
@@ -2172,13 +2172,13 @@
     <row r="9" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F9" s="5" t="b">
         <v>1</v>
@@ -2195,19 +2195,19 @@
     </row>
     <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F10" s="10" t="b">
         <v>1</v>
@@ -2225,13 +2225,13 @@
     <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="C11" s="8" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F11" s="8" t="b">
         <v>1</v>
@@ -2251,19 +2251,19 @@
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F12" s="3" t="b">
         <v>1</v>
@@ -2284,13 +2284,13 @@
     <row r="13" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="C13" s="7" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F13" s="7" t="b">
         <v>1</v>
@@ -2313,16 +2313,16 @@
     </row>
     <row r="14" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F14" s="12" t="b">
         <v>1</v>
@@ -2342,19 +2342,19 @@
     </row>
     <row r="15" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F15" s="13" t="b">
         <v>1</v>
@@ -2363,30 +2363,30 @@
         <v>0</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F16" s="20" t="b">
         <v>1</v>
@@ -2400,19 +2400,19 @@
     </row>
     <row r="17" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F17" s="13" t="b">
         <v>1</v>
@@ -2429,19 +2429,19 @@
     </row>
     <row r="18" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F18" s="20" t="b">
         <v>1</v>
@@ -2486,10 +2486,10 @@
   <sheetData>
     <row r="1" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>5</v>
@@ -2498,31 +2498,31 @@
         <v>2</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F1" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="I1" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="J1" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="K1" s="33" t="s">
-        <v>140</v>
-      </c>
       <c r="L1" s="33" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="M1" s="33" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2530,79 +2530,79 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F7" s="5" t="b">
         <v>1</v>
@@ -2610,16 +2610,16 @@
     </row>
     <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F8" s="10" t="b">
         <v>0</v>
@@ -2630,16 +2630,16 @@
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F9" s="3" t="b">
         <v>0</v>
@@ -2656,16 +2656,16 @@
     </row>
     <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F10" s="10" t="b">
         <v>0</v>
@@ -2683,13 +2683,13 @@
     <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="C11" s="8" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F11" s="8" t="b">
         <v>0</v>
@@ -2706,16 +2706,16 @@
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F12" s="3" t="b">
         <v>0</v>
@@ -2735,16 +2735,16 @@
     </row>
     <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F13" s="10" t="b">
         <v>0</v>
@@ -2767,16 +2767,16 @@
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F14" s="3" t="b">
         <v>0</v>
@@ -2802,16 +2802,16 @@
     </row>
     <row r="15" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F15" s="20" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Improved support for patient workflow testing
- Remove Synthea test patients from Monitoring workflow
- Add patients matching the new workflow spreadsheet
- Add helper python scripts for copying patient resources and pushing resources to FHIR
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBC4F8F8-AEED-A447-A761-6576C860370D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F6432D-4666-D04A-B7F6-849CD5B518F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Adverse Reactions (AR)" sheetId="5" r:id="rId5"/>
     <sheet name="Screening (S)" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="162">
   <si>
     <t>Hypertensive Emergency</t>
   </si>
@@ -491,12 +491,6 @@
     <t>H-RecommendMoreBPs</t>
   </si>
   <si>
-    <t>H-HTNStage2LastBP</t>
-  </si>
-  <si>
-    <t>H-HTNStage2AverageBP</t>
-  </si>
-  <si>
     <t>H-ConsiderHTNStage2</t>
   </si>
   <si>
@@ -513,6 +507,15 @@
   </si>
   <si>
     <t>H-ExcludedOver80</t>
+  </si>
+  <si>
+    <t>H-HTNStage2LastBPSetOffice</t>
+  </si>
+  <si>
+    <t>H-HTNStage2AverageBPOffice</t>
+  </si>
+  <si>
+    <t>H-ConsiderHTNStage2LastBPSetOffice</t>
   </si>
 </sst>
 </file>
@@ -1049,11 +1052,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D39A09-10DC-DF4F-8FB4-83227CE97058}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1123,7 +1126,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
@@ -1302,7 +1305,7 @@
         <v>35</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>6</v>
@@ -1338,7 +1341,7 @@
         <v>35</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>6</v>
@@ -1368,181 +1371,186 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="D13" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="20" t="s">
+      <c r="D16" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F16" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="13" t="s">
+      <c r="H16" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="13" t="s">
+      <c r="D17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F17" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="M14" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="20" t="s">
+      <c r="H17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="M17" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="O17" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="D15" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="20" t="s">
+      <c r="D18" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F18" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" s="20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="M16" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="O16" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="M17" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="N17" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="O17" s="20" t="b">
+      <c r="H18" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M18" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O18" s="20" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Initial Diagnosis patients with Ambulatory procedures.
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1FB2BCD-98FD-CE40-9047-AE634EA7E892}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AC7532-63C5-0148-BAE2-5D40BA8217C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="167">
   <si>
     <t>Hypertensive Emergency</t>
   </si>
@@ -1071,7 +1071,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1392,6 +1392,9 @@
       <c r="C12" s="5" t="s">
         <v>159</v>
       </c>
+      <c r="D12" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="E12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1428,6 +1431,9 @@
       <c r="C13" s="5" t="s">
         <v>163</v>
       </c>
+      <c r="D13" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="E13" s="5" t="s">
         <v>6</v>
       </c>
@@ -1461,6 +1467,9 @@
       <c r="C14" s="5" t="s">
         <v>164</v>
       </c>
+      <c r="D14" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="E14" s="5" t="s">
         <v>6</v>
       </c>
@@ -1494,6 +1503,9 @@
       <c r="C15" s="5" t="s">
         <v>165</v>
       </c>
+      <c r="D15" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="E15" s="5" t="s">
         <v>6</v>
       </c>
@@ -1526,6 +1538,9 @@
       </c>
       <c r="C16" s="7" t="s">
         <v>166</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Initial Diagnosis HTN Stage 1 patients.
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AC7532-63C5-0148-BAE2-5D40BA8217C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2623B9B-0AF3-F241-9B0C-13D8E4D0655C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="167">
   <si>
     <t>Hypertensive Emergency</t>
   </si>
@@ -1071,7 +1071,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1615,6 +1615,9 @@
       <c r="C18" s="13" t="s">
         <v>153</v>
       </c>
+      <c r="D18" s="13" t="s">
+        <v>162</v>
+      </c>
       <c r="E18" s="13" t="s">
         <v>6</v>
       </c>
@@ -1646,6 +1649,9 @@
       </c>
       <c r="C19" s="18" t="s">
         <v>154</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>162</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Clean up bad refs for Logica upload and diversify patient info.
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2623B9B-0AF3-F241-9B0C-13D8E4D0655C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFFE2E3-C75E-1C4A-AB53-3B8C1B0D6159}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="173">
   <si>
     <t>Hypertensive Emergency</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Set Avg &gt; 140 SBP or &gt; 90 DBP</t>
   </si>
   <si>
-    <t>We could further break this down into ambulatory versus office versus home?</t>
-  </si>
-  <si>
     <t>Last &gt; 160 SBP</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Endpoint Description</t>
   </si>
   <si>
-    <t>Note that workflow diagram uses &gt;130/80 but CQL uses &gt;=. Not sure if excluded values will fall to "Patient does not have an indication of hypertensive state" or if that only happens when no further action is needed at the end.</t>
-  </si>
-  <si>
     <t>Prescribe Ambulatory BP Monitoring</t>
   </si>
   <si>
@@ -531,6 +525,30 @@
   </si>
   <si>
     <t>H-HTNStage2AverageBPSetAmbulatory</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Note that workflow diagram uses &gt;130/80 but CQL uses &gt;=</t>
+  </si>
+  <si>
+    <t>Patient diagnosed with HTN Stage 2 based on the average of the last set of office BP readings</t>
+  </si>
+  <si>
+    <t>Patient diagnosed with HTN Stage 2 based on the average of all BP readings in last 2 years where the last set of office readings is not high enough</t>
+  </si>
+  <si>
+    <t>Patient diagnosed with HTN Stage 2 based on the average of the last set of home BP readings</t>
+  </si>
+  <si>
+    <t>Patient diagnosed with HTN Stage 2 based on the average of all BP readings in last 2 years where the last set of home readings is not high enough</t>
+  </si>
+  <si>
+    <t>Patient diagnosed with HTN Stage 2 based on the average of the last set of BP readings related to an Ambulatory Procedure lasting more than 12 hours</t>
+  </si>
+  <si>
+    <t>Patient diagnoses with HTN Stage 2 based on the average of all BP readings in last 2 years where the last set of ambulatory readings is not high enough</t>
   </si>
 </sst>
 </file>
@@ -1071,14 +1089,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="33.1640625" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.6640625" customWidth="1"/>
     <col min="10" max="10" width="29.6640625" bestFit="1" customWidth="1"/>
@@ -1089,16 +1108,16 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1116,28 +1135,28 @@
         <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1145,10 +1164,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
@@ -1160,16 +1179,16 @@
         <v>17</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>42</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>4</v>
@@ -1184,13 +1203,13 @@
     <row r="4" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>6</v>
@@ -1208,13 +1227,13 @@
     <row r="5" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>6</v>
@@ -1232,10 +1251,10 @@
     <row r="6" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>6</v>
@@ -1252,13 +1271,13 @@
         <v>0</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>6</v>
@@ -1273,13 +1292,13 @@
     <row r="8" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>6</v>
@@ -1296,13 +1315,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>6</v>
@@ -1319,16 +1338,16 @@
     </row>
     <row r="10" spans="1:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E10" s="34" t="s">
         <v>6</v>
@@ -1345,16 +1364,16 @@
     </row>
     <row r="11" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>6</v>
@@ -1381,19 +1400,19 @@
         <v>0</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>25</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>6</v>
@@ -1420,19 +1439,19 @@
         <v>1</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>25</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>6</v>
@@ -1457,18 +1476,21 @@
       </c>
       <c r="M13" s="5" t="b">
         <v>0</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>6</v>
@@ -1493,18 +1515,21 @@
       </c>
       <c r="M14" s="5" t="b">
         <v>1</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>6</v>
@@ -1529,18 +1554,21 @@
       </c>
       <c r="M15" s="5" t="b">
         <v>0</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>6</v>
@@ -1566,19 +1594,22 @@
       <c r="M16" s="7" t="b">
         <v>1</v>
       </c>
+      <c r="Q16" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="17" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>6</v>
@@ -1607,16 +1638,16 @@
     </row>
     <row r="18" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>6</v>
@@ -1642,16 +1673,16 @@
     </row>
     <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>6</v>
@@ -1680,13 +1711,16 @@
     </row>
     <row r="20" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>160</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>6</v>
@@ -1718,13 +1752,16 @@
     </row>
     <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>156</v>
+        <v>154</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>160</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>6</v>
@@ -1785,10 +1822,10 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -1806,22 +1843,22 @@
         <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="19" t="s">
         <v>12</v>
@@ -1832,7 +1869,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
@@ -1848,7 +1885,7 @@
     <row r="3" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
@@ -1864,10 +1901,10 @@
     <row r="4" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
@@ -1886,10 +1923,10 @@
     <row r="5" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
@@ -1908,7 +1945,7 @@
     <row r="6" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>6</v>
@@ -1924,7 +1961,7 @@
     <row r="7" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>6</v>
@@ -1936,19 +1973,19 @@
         <v>17</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q7" s="22"/>
     </row>
     <row r="8" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>6</v>
@@ -1960,7 +1997,7 @@
         <v>17</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H8" s="18" t="b">
         <v>0</v>
@@ -1969,13 +2006,13 @@
     </row>
     <row r="9" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>6</v>
@@ -1987,7 +2024,7 @@
         <v>17</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H9" s="13" t="b">
         <v>1</v>
@@ -1999,13 +2036,13 @@
     </row>
     <row r="10" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>6</v>
@@ -2017,7 +2054,7 @@
         <v>17</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H10" s="10" t="b">
         <v>1</v>
@@ -2033,10 +2070,10 @@
     <row r="11" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>6</v>
@@ -2048,7 +2085,7 @@
         <v>17</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H11" s="12" t="b">
         <v>1</v>
@@ -2066,13 +2103,13 @@
     </row>
     <row r="12" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>6</v>
@@ -2084,7 +2121,7 @@
         <v>17</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H12" s="13" t="b">
         <v>1</v>
@@ -2105,13 +2142,13 @@
     </row>
     <row r="13" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>58</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>60</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>6</v>
@@ -2123,7 +2160,7 @@
         <v>17</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H13" s="18" t="b">
         <v>1</v>
@@ -2147,13 +2184,13 @@
     </row>
     <row r="14" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>61</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>6</v>
@@ -2165,7 +2202,7 @@
         <v>17</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H14" s="13" t="b">
         <v>1</v>
@@ -2218,10 +2255,10 @@
   <sheetData>
     <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -2233,25 +2270,25 @@
         <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M1" s="19" t="s">
         <v>12</v>
@@ -2262,89 +2299,89 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M2" s="20"/>
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M3" s="21"/>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M4" s="21"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M5" s="21"/>
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M6" s="22"/>
     </row>
     <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" s="10" t="b">
         <v>0</v>
@@ -2353,19 +2390,19 @@
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F8" s="3" t="b">
         <v>1</v>
@@ -2380,13 +2417,13 @@
     <row r="9" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F9" s="5" t="b">
         <v>1</v>
@@ -2403,19 +2440,19 @@
     </row>
     <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F10" s="10" t="b">
         <v>1</v>
@@ -2433,13 +2470,13 @@
     <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="C11" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F11" s="8" t="b">
         <v>1</v>
@@ -2459,19 +2496,19 @@
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F12" s="3" t="b">
         <v>1</v>
@@ -2492,13 +2529,13 @@
     <row r="13" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="C13" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F13" s="7" t="b">
         <v>1</v>
@@ -2521,16 +2558,16 @@
     </row>
     <row r="14" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F14" s="12" t="b">
         <v>1</v>
@@ -2550,19 +2587,19 @@
     </row>
     <row r="15" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F15" s="13" t="b">
         <v>1</v>
@@ -2571,30 +2608,30 @@
         <v>0</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F16" s="18" t="b">
         <v>1</v>
@@ -2608,19 +2645,19 @@
     </row>
     <row r="17" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F17" s="13" t="b">
         <v>1</v>
@@ -2637,19 +2674,19 @@
     </row>
     <row r="18" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F18" s="18" t="b">
         <v>1</v>
@@ -2694,10 +2731,10 @@
   <sheetData>
     <row r="1" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>5</v>
@@ -2709,28 +2746,28 @@
         <v>21</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I1" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="31" t="s">
-        <v>122</v>
-      </c>
       <c r="K1" s="31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L1" s="31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="M1" s="31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2738,79 +2775,79 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" s="5" t="b">
         <v>1</v>
@@ -2818,16 +2855,16 @@
     </row>
     <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F8" s="10" t="b">
         <v>0</v>
@@ -2838,16 +2875,16 @@
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F9" s="3" t="b">
         <v>0</v>
@@ -2864,16 +2901,16 @@
     </row>
     <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F10" s="10" t="b">
         <v>0</v>
@@ -2891,13 +2928,13 @@
     <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="C11" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F11" s="8" t="b">
         <v>0</v>
@@ -2914,16 +2951,16 @@
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F12" s="3" t="b">
         <v>0</v>
@@ -2943,16 +2980,16 @@
     </row>
     <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F13" s="10" t="b">
         <v>0</v>
@@ -2975,16 +3012,16 @@
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F14" s="3" t="b">
         <v>0</v>
@@ -3010,16 +3047,16 @@
     </row>
     <row r="15" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F15" s="18" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Complete patients for Monitoring workflow.
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFFE2E3-C75E-1C4A-AB53-3B8C1B0D6159}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EB8B1E-AB18-F448-BDF7-DD1552CEC7F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
+    <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" activeTab="1" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
   <sheets>
     <sheet name="Hypertension Initial Dx (H)" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="173">
   <si>
     <t>Hypertensive Emergency</t>
   </si>
@@ -167,9 +167,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>M-RecommendMoreBPsMissingData</t>
-  </si>
-  <si>
     <t>Last or Set Avg BP &gt; 140 SBP or &gt; 90 DBP</t>
   </si>
   <si>
@@ -188,12 +185,6 @@
     <t>Not At Goal: Recommend Treatment</t>
   </si>
   <si>
-    <t>M-NotAtGoalOver140/90</t>
-  </si>
-  <si>
-    <t>M-NotAtGoalOverGoal</t>
-  </si>
-  <si>
     <t>Last or Set Avg BP &gt; 130 SBP or &gt; 80 DBP</t>
   </si>
   <si>
@@ -549,6 +540,15 @@
   </si>
   <si>
     <t>Patient diagnoses with HTN Stage 2 based on the average of all BP readings in last 2 years where the last set of ambulatory readings is not high enough</t>
+  </si>
+  <si>
+    <t>M-NotAtGoalHTNStage2</t>
+  </si>
+  <si>
+    <t>M-NotAtGoalAboveGoal</t>
+  </si>
+  <si>
+    <t>M-RecommendMoreBPs</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D39A09-10DC-DF4F-8FB4-83227CE97058}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
@@ -1117,7 +1117,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1135,7 +1135,7 @@
         <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>24</v>
@@ -1156,7 +1156,7 @@
         <v>42</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1164,10 +1164,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
@@ -1179,16 +1179,16 @@
         <v>17</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>4</v>
@@ -1206,10 +1206,10 @@
         <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>6</v>
@@ -1230,10 +1230,10 @@
         <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>6</v>
@@ -1251,10 +1251,10 @@
     <row r="6" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>6</v>
@@ -1274,10 +1274,10 @@
         <v>30</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>6</v>
@@ -1295,10 +1295,10 @@
         <v>30</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>6</v>
@@ -1318,10 +1318,10 @@
         <v>31</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>6</v>
@@ -1344,10 +1344,10 @@
         <v>32</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E10" s="34" t="s">
         <v>6</v>
@@ -1370,10 +1370,10 @@
         <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>6</v>
@@ -1400,7 +1400,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1409,10 +1409,10 @@
         <v>33</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>6</v>
@@ -1439,7 +1439,7 @@
         <v>1</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1448,10 +1448,10 @@
         <v>33</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>6</v>
@@ -1478,7 +1478,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1487,10 +1487,10 @@
         <v>33</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>6</v>
@@ -1517,7 +1517,7 @@
         <v>1</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1526,10 +1526,10 @@
         <v>33</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>6</v>
@@ -1556,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1565,10 +1565,10 @@
         <v>33</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>6</v>
@@ -1595,7 +1595,7 @@
         <v>1</v>
       </c>
       <c r="Q16" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -1606,10 +1606,10 @@
         <v>34</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>6</v>
@@ -1644,10 +1644,10 @@
         <v>35</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>6</v>
@@ -1679,10 +1679,10 @@
         <v>37</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>6</v>
@@ -1717,10 +1717,10 @@
         <v>41</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>6</v>
@@ -1758,10 +1758,10 @@
         <v>44</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>6</v>
@@ -1798,10 +1798,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4CDD08-6F02-CF4A-8EC8-B1E79A7B6CED}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1809,18 +1809,19 @@
     <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="114.6640625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="6" width="32" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="114.6640625" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1831,180 +1832,204 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="R1" s="19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="20"/>
-    </row>
-    <row r="3" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R2" s="20"/>
+    </row>
+    <row r="3" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="21"/>
-    </row>
-    <row r="4" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R3" s="21"/>
+    </row>
+    <row r="4" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="21"/>
-    </row>
-    <row r="5" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R4" s="21"/>
+    </row>
+    <row r="5" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="21"/>
-    </row>
-    <row r="6" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R5" s="21"/>
+    </row>
+    <row r="6" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Q6" s="21"/>
-    </row>
-    <row r="7" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R6" s="21"/>
+    </row>
+    <row r="7" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q7" s="22"/>
-    </row>
-    <row r="8" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="R7" s="22"/>
+    </row>
+    <row r="8" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E8" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="G8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="24"/>
-    </row>
-    <row r="9" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8" s="24"/>
+    </row>
+    <row r="9" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>39</v>
       </c>
@@ -2012,52 +2037,55 @@
         <v>32</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>45</v>
+        <v>172</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="G9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H9" s="13" t="b">
-        <v>1</v>
+      <c r="H9" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="I9" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="25"/>
-    </row>
-    <row r="10" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="R9" s="25"/>
+    </row>
+    <row r="10" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="10" t="b">
-        <v>1</v>
+      <c r="H10" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="I10" s="10" t="b">
         <v>1</v>
@@ -2065,111 +2093,120 @@
       <c r="J10" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="Q10" s="26"/>
-    </row>
-    <row r="11" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K10" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="R10" s="26"/>
+    </row>
+    <row r="11" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>53</v>
+        <v>171</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="G11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="12" t="b">
-        <v>1</v>
+      <c r="H11" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="I11" s="12" t="b">
         <v>1</v>
       </c>
       <c r="J11" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="27"/>
-    </row>
-    <row r="12" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R11" s="27"/>
+    </row>
+    <row r="12" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="G12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="13" t="b">
-        <v>1</v>
+      <c r="H12" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="I12" s="13" t="b">
         <v>1</v>
       </c>
       <c r="J12" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="13" t="b">
         <v>0</v>
       </c>
       <c r="L12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="25"/>
-    </row>
-    <row r="13" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="R12" s="25"/>
+    </row>
+    <row r="13" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E13" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="G13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="H13" s="18" t="b">
-        <v>1</v>
+      <c r="H13" s="18" t="s">
+        <v>63</v>
       </c>
       <c r="I13" s="18" t="b">
         <v>1</v>
       </c>
       <c r="J13" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="18" t="b">
         <v>0</v>
@@ -2178,40 +2215,43 @@
         <v>0</v>
       </c>
       <c r="M13" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="24"/>
-    </row>
-    <row r="14" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="R13" s="24"/>
+    </row>
+    <row r="14" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>44</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="G14" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="13" t="b">
-        <v>1</v>
+      <c r="H14" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="I14" s="13" t="b">
         <v>1</v>
       </c>
       <c r="J14" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="13" t="b">
         <v>0</v>
@@ -2222,7 +2262,10 @@
       <c r="M14" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="Q14" s="25"/>
+      <c r="N14" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="R14" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2270,25 +2313,25 @@
         <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M1" s="19" t="s">
         <v>12</v>
@@ -2299,26 +2342,26 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M2" s="20"/>
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M3" s="21"/>
     </row>
@@ -2328,13 +2371,13 @@
         <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="M4" s="21"/>
     </row>
@@ -2344,44 +2387,44 @@
         <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M5" s="21"/>
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M6" s="22"/>
     </row>
     <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F7" s="10" t="b">
         <v>0</v>
@@ -2390,19 +2433,19 @@
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F8" s="3" t="b">
         <v>1</v>
@@ -2417,13 +2460,13 @@
     <row r="9" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F9" s="5" t="b">
         <v>1</v>
@@ -2440,19 +2483,19 @@
     </row>
     <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F10" s="10" t="b">
         <v>1</v>
@@ -2470,13 +2513,13 @@
     <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="C11" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F11" s="8" t="b">
         <v>1</v>
@@ -2496,19 +2539,19 @@
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F12" s="3" t="b">
         <v>1</v>
@@ -2529,13 +2572,13 @@
     <row r="13" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="C13" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F13" s="7" t="b">
         <v>1</v>
@@ -2558,16 +2601,16 @@
     </row>
     <row r="14" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F14" s="12" t="b">
         <v>1</v>
@@ -2587,19 +2630,19 @@
     </row>
     <row r="15" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F15" s="13" t="b">
         <v>1</v>
@@ -2608,30 +2651,30 @@
         <v>0</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>97</v>
-      </c>
       <c r="D16" s="18" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F16" s="18" t="b">
         <v>1</v>
@@ -2645,19 +2688,19 @@
     </row>
     <row r="17" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F17" s="13" t="b">
         <v>1</v>
@@ -2674,19 +2717,19 @@
     </row>
     <row r="18" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F18" s="18" t="b">
         <v>1</v>
@@ -2746,28 +2789,28 @@
         <v>21</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H1" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="J1" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="K1" s="31" t="s">
-        <v>121</v>
-      </c>
       <c r="L1" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="31" t="s">
         <v>126</v>
-      </c>
-      <c r="M1" s="31" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2775,25 +2818,25 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2802,13 +2845,13 @@
         <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2817,37 +2860,37 @@
         <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F7" s="5" t="b">
         <v>1</v>
@@ -2855,16 +2898,16 @@
     </row>
     <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F8" s="10" t="b">
         <v>0</v>
@@ -2875,16 +2918,16 @@
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F9" s="3" t="b">
         <v>0</v>
@@ -2901,16 +2944,16 @@
     </row>
     <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>122</v>
-      </c>
       <c r="D10" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F10" s="10" t="b">
         <v>0</v>
@@ -2928,13 +2971,13 @@
     <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="C11" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F11" s="8" t="b">
         <v>0</v>
@@ -2951,16 +2994,16 @@
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F12" s="3" t="b">
         <v>0</v>
@@ -2980,16 +3023,16 @@
     </row>
     <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F13" s="10" t="b">
         <v>0</v>
@@ -3012,16 +3055,16 @@
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F14" s="3" t="b">
         <v>0</v>
@@ -3047,16 +3090,16 @@
     </row>
     <row r="15" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F15" s="18" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Delete old non-pharma patients and add excluded cases.
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EB8B1E-AB18-F448-BDF7-DD1552CEC7F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA255155-C3A6-8744-8849-C087A882C3FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" activeTab="1" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
+    <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" activeTab="2" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
   <sheets>
     <sheet name="Hypertension Initial Dx (H)" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="173">
   <si>
     <t>Hypertensive Emergency</t>
   </si>
@@ -1800,7 +1800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4CDD08-6F02-CF4A-8EC8-B1E79A7B6CED}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -2274,10 +2274,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D635F18-F41B-2147-9020-03D985935021}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2285,18 +2285,19 @@
     <col min="1" max="1" width="37.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.5" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.6640625" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.6640625" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -2307,37 +2308,40 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="N1" s="19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2345,27 +2349,33 @@
         <v>66</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="M2" s="20"/>
-    </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N2" s="20"/>
+    </row>
+    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
         <v>67</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="21"/>
-    </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N3" s="21"/>
+    </row>
+    <row r="4" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>28</v>
@@ -2373,15 +2383,15 @@
       <c r="C4" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="M4" s="21"/>
-    </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N4" s="21"/>
+    </row>
+    <row r="5" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
         <v>29</v>
@@ -2390,27 +2400,33 @@
         <v>69</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="21"/>
-    </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N5" s="21"/>
+    </row>
+    <row r="6" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="C6" s="7" t="s">
         <v>70</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="M6" s="22"/>
-    </row>
-    <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N6" s="22"/>
+    </row>
+    <row r="7" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>46</v>
       </c>
@@ -2420,18 +2436,18 @@
       <c r="C7" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>6</v>
-      </c>
       <c r="E7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" s="26"/>
-    </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G7" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="26"/>
+    </row>
+    <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>74</v>
       </c>
@@ -2441,36 +2457,33 @@
       <c r="C8" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="E8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="G8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="C9" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="E9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="5" t="b">
-        <v>1</v>
-      </c>
       <c r="G9" s="5" t="b">
         <v>1</v>
       </c>
@@ -2480,8 +2493,11 @@
       <c r="I9" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J9" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>79</v>
       </c>
@@ -2491,39 +2507,36 @@
       <c r="C10" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>6</v>
-      </c>
       <c r="E10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="10" t="b">
-        <v>1</v>
-      </c>
       <c r="G10" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10" t="b">
         <v>0</v>
       </c>
       <c r="J10" s="10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="C11" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>6</v>
-      </c>
       <c r="E11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="G11" s="8" t="b">
         <v>1</v>
       </c>
@@ -2531,13 +2544,16 @@
         <v>1</v>
       </c>
       <c r="I11" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>82</v>
       </c>
@@ -2547,42 +2563,39 @@
       <c r="C12" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="G12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3" t="b">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="b">
         <v>0</v>
       </c>
       <c r="K12" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="C13" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>6</v>
-      </c>
       <c r="E13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="7" t="b">
-        <v>1</v>
-      </c>
       <c r="G13" s="7" t="b">
         <v>1</v>
       </c>
@@ -2590,36 +2603,36 @@
         <v>1</v>
       </c>
       <c r="I13" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="7" t="b">
         <v>0</v>
       </c>
       <c r="K13" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>85</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>6</v>
-      </c>
       <c r="E14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="12" t="b">
-        <v>1</v>
-      </c>
       <c r="G14" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="12" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="H14" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="J14" s="12" t="b">
         <v>1</v>
@@ -2627,8 +2640,11 @@
       <c r="K14" s="12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L14" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>89</v>
       </c>
@@ -2638,20 +2654,17 @@
       <c r="C15" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>6</v>
-      </c>
       <c r="E15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="13" t="b">
-        <v>1</v>
-      </c>
       <c r="G15" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>90</v>
+        <v>1</v>
+      </c>
+      <c r="H15" s="13" t="b">
+        <v>0</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>90</v>
@@ -2659,8 +2672,11 @@
       <c r="K15" s="13" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L15" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>91</v>
       </c>
@@ -2670,23 +2686,23 @@
       <c r="C16" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>6</v>
-      </c>
       <c r="E16" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="18" t="b">
-        <v>1</v>
-      </c>
       <c r="G16" s="18" t="b">
         <v>1</v>
       </c>
       <c r="H16" s="18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>97</v>
       </c>
@@ -2696,26 +2712,26 @@
       <c r="C17" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>6</v>
-      </c>
       <c r="E17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="13" t="b">
-        <v>1</v>
-      </c>
       <c r="G17" s="13" t="b">
         <v>1</v>
       </c>
       <c r="H17" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17" s="13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="M17" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>100</v>
       </c>
@@ -2725,22 +2741,22 @@
       <c r="C18" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>6</v>
-      </c>
       <c r="E18" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="18" t="b">
-        <v>1</v>
-      </c>
       <c r="G18" s="18" t="b">
         <v>1</v>
       </c>
       <c r="H18" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="M18" s="18" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Complete NonPharma patients needing counseling.
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA255155-C3A6-8744-8849-C087A882C3FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2409B20F-FA22-1045-B712-E1750B987D0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" activeTab="2" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="176">
   <si>
     <t>Hypertensive Emergency</t>
   </si>
@@ -549,6 +549,15 @@
   </si>
   <si>
     <t>M-RecommendMoreBPs</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>This doesn't work currently and highlights a hole in logic. The patient previously had counseling for BMI and saw improvement. In the meantime, drinking has increased, but they do not get recommended for counseling because their previous counseling was not specific to drinking.</t>
+  </si>
+  <si>
+    <t>Pregnancy has no time constraints, so a person is currently always excluded from the intervention if they were ever pregnant.</t>
   </si>
 </sst>
 </file>
@@ -572,7 +581,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,6 +609,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,7 +732,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -771,6 +786,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2276,8 +2301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D635F18-F41B-2147-9020-03D985935021}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2294,7 +2319,7 @@
     <col min="11" max="11" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="35.6640625" customWidth="1"/>
-    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2375,21 +2400,26 @@
       </c>
       <c r="N3" s="21"/>
     </row>
-    <row r="4" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:14" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="35"/>
+      <c r="B4" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="D4" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="N4" s="21"/>
+      <c r="N4" s="37" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="5" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
@@ -2436,6 +2466,9 @@
       <c r="C7" s="10" t="s">
         <v>71</v>
       </c>
+      <c r="D7" s="10" t="s">
+        <v>157</v>
+      </c>
       <c r="E7" s="10" t="s">
         <v>6</v>
       </c>
@@ -2456,6 +2489,9 @@
       </c>
       <c r="C8" s="3" t="s">
         <v>76</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>6</v>
@@ -2478,6 +2514,9 @@
       <c r="C9" s="5" t="s">
         <v>77</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>157</v>
+      </c>
       <c r="E9" s="5" t="s">
         <v>6</v>
       </c>
@@ -2506,6 +2545,9 @@
       </c>
       <c r="C10" s="10" t="s">
         <v>80</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>157</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>6</v>
@@ -2531,6 +2573,9 @@
       <c r="C11" s="8" t="s">
         <v>81</v>
       </c>
+      <c r="D11" s="8" t="s">
+        <v>157</v>
+      </c>
       <c r="E11" s="8" t="s">
         <v>6</v>
       </c>
@@ -2563,6 +2608,9 @@
       <c r="C12" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>157</v>
+      </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
       </c>
@@ -2585,34 +2633,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="C13" s="7" t="s">
+    <row r="13" spans="1:14" s="39" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A13" s="38"/>
+      <c r="C13" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="7" t="s">
+      <c r="D13" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13" s="7" t="b">
-        <v>1</v>
+      <c r="G13" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" s="40" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -2621,6 +2675,9 @@
       </c>
       <c r="C14" s="12" t="s">
         <v>86</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Complete patients for NonPharma workflow.
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2409B20F-FA22-1045-B712-E1750B987D0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB89B9B8-7726-A742-8771-4F86D29B366A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" activeTab="2" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="177">
   <si>
     <t>Hypertensive Emergency</t>
   </si>
@@ -557,7 +557,10 @@
     <t>This doesn't work currently and highlights a hole in logic. The patient previously had counseling for BMI and saw improvement. In the meantime, drinking has increased, but they do not get recommended for counseling because their previous counseling was not specific to drinking.</t>
   </si>
   <si>
-    <t>Pregnancy has no time constraints, so a person is currently always excluded from the intervention if they were ever pregnant.</t>
+    <t>NPI-SmokingCessationQuit</t>
+  </si>
+  <si>
+    <t>Current logic does not handle a patient who previously smoked but has a more recent observation indicating they are a former smoker</t>
   </si>
 </sst>
 </file>
@@ -732,7 +735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -788,9 +791,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2299,10 +2299,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D635F18-F41B-2147-9020-03D985935021}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2400,26 +2400,24 @@
       </c>
       <c r="N3" s="21"/>
     </row>
-    <row r="4" spans="1:14" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36" t="s">
+    <row r="4" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="36" t="s">
+      <c r="D4" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="N4" s="37" t="s">
-        <v>175</v>
-      </c>
+      <c r="N4" s="21"/>
     </row>
     <row r="5" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
@@ -2536,284 +2534,323 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="35"/>
+      <c r="C10" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="36" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B11" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="D11" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" s="10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="C11" s="8" t="s">
+      <c r="G11" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14"/>
+      <c r="C12" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="D12" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="G12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="D13" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="39" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A13" s="38"/>
-      <c r="C13" s="39" t="s">
+      <c r="G13" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="38" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A14" s="37"/>
+      <c r="C14" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D14" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="E13" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="39" t="s">
+      <c r="E14" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" s="40" t="s">
+      <c r="G14" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" s="39" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+    <row r="15" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C15" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="12" t="s">
+      <c r="D15" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L14" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+      <c r="G15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L15" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B16" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C16" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="13" t="s">
+      <c r="D16" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="13" t="s">
+      <c r="G16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K15" s="13" t="s">
+      <c r="K16" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="L16" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
+    <row r="17" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B17" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C17" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="18" t="s">
+      <c r="D17" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" s="18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="G17" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B18" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C18" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="13" t="s">
+      <c r="D18" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="M17" s="13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
+      <c r="G18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="M18" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B19" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C19" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="18" t="s">
+      <c r="D19" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="M18" s="18" t="b">
+      <c r="G19" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="M19" s="18" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes #8: Handle former smokers with previous smoking observations.
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB89B9B8-7726-A742-8771-4F86D29B366A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CD74D1-6395-8448-B3CF-926EE7EF9BD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" activeTab="2" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
+    <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
   <sheets>
     <sheet name="Hypertension Initial Dx (H)" sheetId="1" r:id="rId1"/>
@@ -1112,9 +1112,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D39A09-10DC-DF4F-8FB4-83227CE97058}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2301,7 +2301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D635F18-F41B-2147-9020-03D985935021}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update NonPharma library with new logic
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CD74D1-6395-8448-B3CF-926EE7EF9BD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2EBC3F-10C6-F94A-A710-21EDAFDFBC7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
+    <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" activeTab="2" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
   <sheets>
     <sheet name="Hypertension Initial Dx (H)" sheetId="1" r:id="rId1"/>
@@ -560,7 +560,7 @@
     <t>NPI-SmokingCessationQuit</t>
   </si>
   <si>
-    <t>Current logic does not handle a patient who previously smoked but has a more recent observation indicating they are a former smoker</t>
+    <t>Fixed in #8</t>
   </si>
 </sst>
 </file>
@@ -735,7 +735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -789,8 +789,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1112,7 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D39A09-10DC-DF4F-8FB4-83227CE97058}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
@@ -2301,8 +2299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D635F18-F41B-2147-9020-03D985935021}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2534,30 +2532,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="35"/>
-      <c r="C10" s="36" t="s">
+    <row r="10" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="C10" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D10" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="E10" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="36" t="s">
+      <c r="D10" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" s="36" t="s">
+      <c r="G10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2658,39 +2656,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="38" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A14" s="37"/>
-      <c r="C14" s="38" t="s">
+    <row r="14" spans="1:14" s="36" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A14" s="35"/>
+      <c r="C14" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="E14" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="38" t="s">
+      <c r="E14" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="38" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" s="38" t="b">
-        <v>0</v>
-      </c>
-      <c r="L14" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="N14" s="39" t="s">
+      <c r="G14" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" s="37" t="s">
         <v>174</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New NonPharma workflow separating behaviors
Implement the new flow diagram that separates recommendations/reminders for different behaviors. This does not yet include any decision logic for physical activity.
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2EBC3F-10C6-F94A-A710-21EDAFDFBC7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6ED4F9-A86C-3940-AB9D-D2D7DD3F2E76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" activeTab="2" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="187">
   <si>
     <t>Hypertensive Emergency</t>
   </si>
@@ -248,27 +248,18 @@
     <t>NPI-SetBPGoalMissingGoal</t>
   </si>
   <si>
-    <t>Previous Non-Pharma Instructions?</t>
-  </si>
-  <si>
     <t>Current smoker?</t>
   </si>
   <si>
     <t>Recommend Smoking Cessation Counseling</t>
   </si>
   <si>
-    <t>Smoking, drinking, weight increase?</t>
-  </si>
-  <si>
     <t>NPI-SmokingCessationNew</t>
   </si>
   <si>
     <t>NPI-SmokingCessationIncrease</t>
   </si>
   <si>
-    <t>BMI &gt; 25?</t>
-  </si>
-  <si>
     <t>Recommend Weight Loss Counseling</t>
   </si>
   <si>
@@ -284,9 +275,6 @@
     <t>NPI-AlcoholModerationNew</t>
   </si>
   <si>
-    <t>Drink Heavily?</t>
-  </si>
-  <si>
     <t>All Counseling Recommended</t>
   </si>
   <si>
@@ -299,24 +287,9 @@
     <t>Not At Goal</t>
   </si>
   <si>
-    <t>Provide Dietary/Physical Activity Counseling</t>
-  </si>
-  <si>
-    <t>any</t>
-  </si>
-  <si>
-    <t>Provide Reminder of Recommendations</t>
-  </si>
-  <si>
     <t>NPI-AlcoholModerationIncrease</t>
   </si>
   <si>
-    <t>NPI-DietActivityCounseling</t>
-  </si>
-  <si>
-    <t>NPI-RecommendationReminder</t>
-  </si>
-  <si>
     <t>Pregnant + Preexisting Hypertension</t>
   </si>
   <si>
@@ -440,9 +413,6 @@
     <t>Patient is in Need of Dietary Counseling Action Path</t>
   </si>
   <si>
-    <t>Patient Reminder Recommendations Action Path</t>
-  </si>
-  <si>
     <t>Patient at BP Goal</t>
   </si>
   <si>
@@ -551,16 +521,76 @@
     <t>M-RecommendMoreBPs</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>This doesn't work currently and highlights a hole in logic. The patient previously had counseling for BMI and saw improvement. In the meantime, drinking has increased, but they do not get recommended for counseling because their previous counseling was not specific to drinking.</t>
-  </si>
-  <si>
     <t>NPI-SmokingCessationQuit</t>
   </si>
   <si>
     <t>Fixed in #8</t>
+  </si>
+  <si>
+    <t>NPI-DietaryCounseling</t>
+  </si>
+  <si>
+    <t>Previous Smoking Counseling?</t>
+  </si>
+  <si>
+    <t>Has smoking increased?</t>
+  </si>
+  <si>
+    <t>BMI&gt;25?</t>
+  </si>
+  <si>
+    <t>Previous Weight Loss Counseling?</t>
+  </si>
+  <si>
+    <t>Has BMI increased?</t>
+  </si>
+  <si>
+    <t>NPI-SmokingCessationReminder</t>
+  </si>
+  <si>
+    <t>Heavy Drinker?</t>
+  </si>
+  <si>
+    <t>Previous Alcohol Counseling?</t>
+  </si>
+  <si>
+    <t>Has drinking increased?</t>
+  </si>
+  <si>
+    <t>Previous Dietary Counseling?</t>
+  </si>
+  <si>
+    <t>Previous Activity Counseling?</t>
+  </si>
+  <si>
+    <t>NPI-WeightLossReminder</t>
+  </si>
+  <si>
+    <t>NPI-WeightLossAchieved</t>
+  </si>
+  <si>
+    <t>NPI-AlcoholModerationReminder</t>
+  </si>
+  <si>
+    <t>Fixed in #9</t>
+  </si>
+  <si>
+    <t>NPI-AlcoholModerationUnrelatedCounseling</t>
+  </si>
+  <si>
+    <t>NPI-AlcoholModerationAchieved</t>
+  </si>
+  <si>
+    <t>Provide Dietary Counseling</t>
+  </si>
+  <si>
+    <t>Provide Activity Counseling</t>
+  </si>
+  <si>
+    <t>Patient is in Need of Activity Counseling Action Path</t>
+  </si>
+  <si>
+    <t>NPI-ActivityCounseling</t>
   </si>
 </sst>
 </file>
@@ -584,7 +614,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,12 +642,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,7 +759,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -789,11 +813,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1140,7 +1159,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1158,7 +1177,7 @@
         <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>24</v>
@@ -1179,7 +1198,7 @@
         <v>42</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1187,10 +1206,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
@@ -1202,16 +1221,16 @@
         <v>17</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>4</v>
@@ -1229,10 +1248,10 @@
         <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>6</v>
@@ -1253,10 +1272,10 @@
         <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>6</v>
@@ -1274,10 +1293,10 @@
     <row r="6" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>6</v>
@@ -1297,10 +1316,10 @@
         <v>30</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>6</v>
@@ -1318,10 +1337,10 @@
         <v>30</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>6</v>
@@ -1341,10 +1360,10 @@
         <v>31</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>6</v>
@@ -1367,10 +1386,10 @@
         <v>32</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E10" s="34" t="s">
         <v>6</v>
@@ -1393,10 +1412,10 @@
         <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>6</v>
@@ -1423,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1432,10 +1451,10 @@
         <v>33</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>6</v>
@@ -1462,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1471,10 +1490,10 @@
         <v>33</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>6</v>
@@ -1501,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1510,10 +1529,10 @@
         <v>33</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>6</v>
@@ -1540,7 +1559,7 @@
         <v>1</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1549,10 +1568,10 @@
         <v>33</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>6</v>
@@ -1579,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1588,10 +1607,10 @@
         <v>33</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>6</v>
@@ -1618,7 +1637,7 @@
         <v>1</v>
       </c>
       <c r="Q16" s="7" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -1629,10 +1648,10 @@
         <v>34</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>6</v>
@@ -1667,10 +1686,10 @@
         <v>35</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>6</v>
@@ -1702,10 +1721,10 @@
         <v>37</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>6</v>
@@ -1740,10 +1759,10 @@
         <v>41</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>6</v>
@@ -1781,10 +1800,10 @@
         <v>44</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>6</v>
@@ -1855,7 +1874,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1899,7 +1918,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
@@ -1918,7 +1937,7 @@
         <v>59</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>4</v>
@@ -1940,7 +1959,7 @@
         <v>60</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>6</v>
@@ -1965,7 +1984,7 @@
         <v>61</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>6</v>
@@ -1987,7 +2006,7 @@
         <v>62</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>6</v>
@@ -2006,7 +2025,7 @@
         <v>64</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>6</v>
@@ -2027,13 +2046,13 @@
         <v>46</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>6</v>
@@ -2060,10 +2079,10 @@
         <v>32</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>6</v>
@@ -2093,10 +2112,10 @@
         <v>33</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>6</v>
@@ -2124,13 +2143,13 @@
     <row r="11" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>6</v>
@@ -2169,7 +2188,7 @@
         <v>57</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>6</v>
@@ -2211,7 +2230,7 @@
         <v>55</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>6</v>
@@ -2256,7 +2275,7 @@
         <v>56</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>6</v>
@@ -2297,10 +2316,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D635F18-F41B-2147-9020-03D985935021}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2311,16 +2332,22 @@
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.5" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.6640625" customWidth="1"/>
-    <col min="14" max="14" width="53.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.6640625" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.6640625" customWidth="1"/>
+    <col min="17" max="17" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.5" customWidth="1"/>
+    <col min="19" max="19" width="35.6640625" customWidth="1"/>
+    <col min="20" max="20" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -2331,7 +2358,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -2346,25 +2373,43 @@
         <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>75</v>
+        <v>166</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>168</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="N1" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="T1" s="19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2372,7 +2417,7 @@
         <v>66</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
@@ -2380,15 +2425,15 @@
       <c r="F2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N2" s="20"/>
-    </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T2" s="20"/>
+    </row>
+    <row r="3" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
         <v>67</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>4</v>
@@ -2396,9 +2441,9 @@
       <c r="F3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N3" s="21"/>
-    </row>
-    <row r="4" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T3" s="21"/>
+    </row>
+    <row r="4" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>28</v>
@@ -2407,17 +2452,17 @@
         <v>68</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="N4" s="21"/>
-    </row>
-    <row r="5" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+      <c r="T4" s="21"/>
+    </row>
+    <row r="5" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
         <v>29</v>
@@ -2426,23 +2471,23 @@
         <v>69</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="N5" s="21"/>
-    </row>
-    <row r="6" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="T5" s="21"/>
+    </row>
+    <row r="6" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="C6" s="7" t="s">
         <v>70</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>6</v>
@@ -2450,20 +2495,20 @@
       <c r="F6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="N6" s="22"/>
-    </row>
-    <row r="7" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T6" s="22"/>
+    </row>
+    <row r="7" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>71</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>6</v>
@@ -2474,20 +2519,20 @@
       <c r="G7" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="N7" s="26"/>
-    </row>
-    <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T7" s="26"/>
+    </row>
+    <row r="8" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>6</v>
@@ -2499,19 +2544,31 @@
         <v>1</v>
       </c>
       <c r="H8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>6</v>
@@ -2531,14 +2588,26 @@
       <c r="J9" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R9" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>6</v>
@@ -2553,302 +2622,599 @@
         <v>1</v>
       </c>
       <c r="I10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R10" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="C11" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14"/>
+      <c r="C13" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="R13" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14"/>
+      <c r="C14" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="R14" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14"/>
+      <c r="C15" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="R15" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B16" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" s="10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="C12" s="8" t="s">
+      <c r="D16" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R16" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="T17" s="21"/>
+    </row>
+    <row r="18" spans="1:20" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="C18" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="T18" s="21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="C19" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N19" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="T19" s="21"/>
+    </row>
+    <row r="20" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="R20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="T20" s="22"/>
+    </row>
+    <row r="21" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="C21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="36" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A14" s="35"/>
-      <c r="C14" s="36" t="s">
+      <c r="D21" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R21" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="N22" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="R22" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="N23" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="R23" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="N24" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="R24" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="S24" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="E14" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="L14" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="N14" s="37" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L15" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="M18" s="13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="M19" s="18" t="b">
+      <c r="D25" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="N25" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="R25" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="S25" s="18" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2897,28 +3263,28 @@
         <v>21</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="G1" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="31" t="s">
-        <v>112</v>
-      </c>
       <c r="I1" s="31" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="J1" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="31" t="s">
         <v>117</v>
-      </c>
-      <c r="K1" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="M1" s="31" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2926,7 +3292,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>3</v>
@@ -2938,7 +3304,7 @@
     <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
@@ -2953,13 +3319,13 @@
         <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2968,19 +3334,19 @@
         <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>6</v>
@@ -2992,7 +3358,7 @@
     <row r="7" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>6</v>
@@ -3006,10 +3372,10 @@
     </row>
     <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>6</v>
@@ -3026,10 +3392,10 @@
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>6</v>
@@ -3052,10 +3418,10 @@
     </row>
     <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>6</v>
@@ -3079,7 +3445,7 @@
     <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="C11" s="8" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>6</v>
@@ -3102,10 +3468,10 @@
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>6</v>
@@ -3131,10 +3497,10 @@
     </row>
     <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>6</v>
@@ -3163,10 +3529,10 @@
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>6</v>
@@ -3198,10 +3564,10 @@
     </row>
     <row r="15" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Remove excluded population from recommendations flow
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6ED4F9-A86C-3940-AB9D-D2D7DD3F2E76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E47A06-5479-C44E-A13E-3E8ADC182D6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" activeTab="2" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
@@ -2321,7 +2321,7 @@
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add Physical Activity value set and workflow logic
Added value set http://cts.nlm.nih.gov/fhir/ValueSet/2.16.840.1.113762.1.4.1116.418 for Physical Activity recommendations. This may not be final.
</commit_message>
<xml_diff>
--- a/specification/HTN_Workflow_Endpoint_Patients.xlsx
+++ b/specification/HTN_Workflow_Endpoint_Patients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E47A06-5479-C44E-A13E-3E8ADC182D6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FA9F00-94CF-3645-8131-116AB4B6F53F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16920" activeTab="2" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="27640" windowHeight="16920" activeTab="2" xr2:uid="{B5FE4CFE-7827-5E4C-BBE4-966466AAED79}"/>
   </bookViews>
   <sheets>
     <sheet name="Hypertension Initial Dx (H)" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="191">
   <si>
     <t>Hypertensive Emergency</t>
   </si>
@@ -581,16 +581,28 @@
     <t>NPI-AlcoholModerationAchieved</t>
   </si>
   <si>
-    <t>Provide Dietary Counseling</t>
-  </si>
-  <si>
-    <t>Provide Activity Counseling</t>
-  </si>
-  <si>
     <t>Patient is in Need of Activity Counseling Action Path</t>
   </si>
   <si>
     <t>NPI-ActivityCounseling</t>
+  </si>
+  <si>
+    <t>Dietary Counseling</t>
+  </si>
+  <si>
+    <t>NOT Patient is in Need of Dietary Counseling Action Path</t>
+  </si>
+  <si>
+    <t>NPI-DietaryReminder</t>
+  </si>
+  <si>
+    <t>Activity Counseling</t>
+  </si>
+  <si>
+    <t>NOT Patient is in Need of Activity Counseling Action Path</t>
+  </si>
+  <si>
+    <t>NPI-ActivityReminder</t>
   </si>
 </sst>
 </file>
@@ -2316,18 +2328,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D635F18-F41B-2147-9020-03D985935021}">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="5.83203125" bestFit="1" customWidth="1"/>
@@ -3013,208 +3025,281 @@
       </c>
       <c r="T20" s="22"/>
     </row>
-    <row r="21" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L21" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N21" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="O21" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="R21" s="12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
+      <c r="D21" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="R21" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R22" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N23" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="R23" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="N22" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="R22" s="13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
+      <c r="C24" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K23" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="N23" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="R23" s="18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
+      <c r="D24" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="N24" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="R24" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N25" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R25" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B26" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C26" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G24" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K24" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="N24" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="R24" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="S24" s="13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
+      <c r="D26" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="R26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="S26" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B27" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C27" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H25" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="K25" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="N25" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="R25" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="S25" s="18" t="b">
+      <c r="D27" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="N27" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="R27" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="S27" s="18" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>